<commit_message>
add code for tables
</commit_message>
<xml_diff>
--- a/Documents/Data_Codebook.xlsx
+++ b/Documents/Data_Codebook.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8184E10B-8139-4D5C-985B-4C408EE4933D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D52D60E-F344-429F-8EF6-890BE5D1A1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1290" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -557,9 +557,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -571,6 +568,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,21 +854,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F20" sqref="F20"/>
+      <selection pane="topRight" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" style="12" customWidth="1"/>
     <col min="2" max="2" width="23.109375" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="53.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -882,7 +882,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -894,7 +894,7 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -904,7 +904,7 @@
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -916,7 +916,7 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -928,39 +928,39 @@
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="9"/>
+      <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="13"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -972,7 +972,7 @@
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -984,7 +984,7 @@
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -996,7 +996,7 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1008,21 +1008,21 @@
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="11">
+      <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="11">
+      <c r="A14" s="10">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1033,7 +1033,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="11">
+      <c r="A15" s="10">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1044,21 +1044,21 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="11">
+      <c r="A16" s="10">
         <v>15</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="11">
+      <c r="A17" s="10">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1069,7 +1069,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="11">
+      <c r="A18" s="10">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1083,7 +1083,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="11">
+      <c r="A19" s="10">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1097,7 +1097,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="11">
+      <c r="A20" s="10">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1111,7 +1111,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
+      <c r="A21" s="10">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -1125,7 +1125,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="11">
+      <c r="A22" s="10">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
@@ -1139,7 +1139,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="11">
+      <c r="A23" s="10">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
@@ -1153,7 +1153,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="11">
+      <c r="A24" s="10">
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -1167,7 +1167,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="11">
+      <c r="A25" s="10">
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -1179,7 +1179,7 @@
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A26" s="11">
+      <c r="A26" s="10">
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -1193,7 +1193,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="11">
+      <c r="A27" s="10">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1207,7 +1207,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="11">
+      <c r="A28" s="10">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1221,7 +1221,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="11">
+      <c r="A29" s="10">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1235,7 +1235,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="11">
+      <c r="A30" s="10">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1249,7 +1249,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="11">
+      <c r="A31" s="10">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1263,7 +1263,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="11">
+      <c r="A32" s="10">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1277,7 +1277,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="11">
+      <c r="A33" s="10">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1291,7 +1291,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="11">
+      <c r="A34" s="10">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1305,7 +1305,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="11">
+      <c r="A35" s="10">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1319,7 +1319,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="11">
+      <c r="A36" s="10">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -1333,7 +1333,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="11">
+      <c r="A37" s="10">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1347,7 +1347,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="11">
+      <c r="A38" s="10">
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
@@ -1361,7 +1361,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="11">
+      <c r="A39" s="10">
         <v>38</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -1373,7 +1373,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="11">
+      <c r="A40" s="10">
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -1385,7 +1385,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="11">
+      <c r="A41" s="10">
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
@@ -1397,7 +1397,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="11">
+      <c r="A42" s="10">
         <v>41</v>
       </c>
       <c r="B42" s="8" t="s">
@@ -1411,7 +1411,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="11">
+      <c r="A43" s="10">
         <v>42</v>
       </c>
       <c r="B43" s="8" t="s">
@@ -1425,7 +1425,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="11">
+      <c r="A44" s="10">
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
@@ -1439,7 +1439,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="11">
+      <c r="A45" s="10">
         <v>44</v>
       </c>
       <c r="B45" s="7" t="s">
@@ -1449,7 +1449,7 @@
       <c r="D45" s="7"/>
     </row>
     <row r="46" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="11">
+      <c r="A46" s="10">
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
@@ -1461,7 +1461,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="11">
+      <c r="A47" s="10">
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
@@ -1473,7 +1473,7 @@
       <c r="D47" s="8"/>
     </row>
     <row r="48" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="11">
+      <c r="A48" s="10">
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
@@ -1487,7 +1487,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="11">
+      <c r="A49" s="10">
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
@@ -1497,7 +1497,7 @@
       <c r="D49" s="7"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="11">
+      <c r="A50" s="10">
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
@@ -1511,7 +1511,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="11">
+      <c r="A51" s="10">
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
@@ -1525,7 +1525,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="11">
+      <c r="A52" s="10">
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
@@ -1537,7 +1537,7 @@
       <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A53" s="11">
+      <c r="A53" s="10">
         <v>52</v>
       </c>
       <c r="B53" s="7" t="s">
@@ -1551,7 +1551,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="69" x14ac:dyDescent="0.3">
-      <c r="A54" s="11">
+      <c r="A54" s="10">
         <v>53</v>
       </c>
       <c r="B54" s="7" t="s">
@@ -1565,7 +1565,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="11">
+      <c r="A55" s="10">
         <v>54</v>
       </c>
       <c r="B55" s="7" t="s">
@@ -1579,7 +1579,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="11">
+      <c r="A56" s="10">
         <v>55</v>
       </c>
       <c r="B56" s="7" t="s">
@@ -1593,7 +1593,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="11">
+      <c r="A57" s="10">
         <v>56</v>
       </c>
       <c r="B57" s="7" t="s">
@@ -1607,7 +1607,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="11">
+      <c r="A58" s="10">
         <v>57</v>
       </c>
       <c r="B58" s="7" t="s">
@@ -1621,7 +1621,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="11">
+      <c r="A59" s="10">
         <v>58</v>
       </c>
       <c r="B59" s="7" t="s">

</xml_diff>